<commit_message>
ASA count update & UI container update
</commit_message>
<xml_diff>
--- a/application/asa/locale.xlsx
+++ b/application/asa/locale.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
   <si>
     <t>ko</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,223 +64,279 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Connection Success</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Setting %s with %s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connection Failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Incorrect Setting %s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Register ASA Domain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connect ASA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASA Domain Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASA Address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Admin ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique Name Required</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Domain Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ASA IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+Administrator ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+Start Connections</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+Max Connections</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연결 성공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%s 가 %s 로 설정되었습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연결 실패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%s 와 연결이 실패하였습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASA 도메인 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASA 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASA 도메인 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASA 주소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>암호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고유한 이름을 입력하세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도메인 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+관리자 ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+시작 연결 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+최대 연결 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-exist ASA Connection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASA 연결이 없습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System Utilization History</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간별 시스템 사용률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System Current</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 시스템 사용률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>From</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Original</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Translate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trans-Hits</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Untrans-Hits</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설정방식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원본주소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경주소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경수치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미변경수치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connection Counts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연결 수치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Translation Counts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경 정보 수치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>counts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연결됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최대치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connections</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커넥션 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Translations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경작업 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Counts</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Connection Success</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Setting %s with %s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Connection Failed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Incorrect Setting %s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Register ASA Domain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Connect ASA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASA Domain Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASA Address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Admin ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unique Name Required</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Domain Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+ASA IP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+Administrator ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+Start Connections</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+Max Connections</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연결 성공</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%s 가 %s 로 설정되었습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연결 실패</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%s 와 연결이 실패하였습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASA 도메인 등록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASA 연결</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASA 도메인 이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASA 주소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>암호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고유한 이름을 입력하세요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도메인 이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+관리자 ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+시작 연결 개수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+최대 연결 개수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Non-exist ASA Connection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASA 연결이 없습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System Utilization History</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간별 시스템 사용률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System Current</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>현재 시스템 사용률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>할당됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Config</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>From</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>To</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Original</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Translate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trans-Hits</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Untrans-Hits</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설정방식</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>입력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>원본주소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>변경주소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>변경수치</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미변경수치</t>
+    <t>수치정보</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -655,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -698,441 +754,539 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D22">
-    <sortCondition ref="A2:A22"/>
+  <sortState ref="A2:D35">
+    <sortCondition ref="A2:A35"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update ASA & Performance Enhancing
</commit_message>
<xml_diff>
--- a/application/asa/locale.xlsx
+++ b/application/asa/locale.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="131">
   <si>
     <t>ko</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -337,6 +337,206 @@
   </si>
   <si>
     <t>수치정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Domain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도메인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Register Success</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록 성공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%s/%s to %s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%s/%s 가 %s로 등록 되었습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Register Failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록 실패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Incorrect Setting %s/%s to %s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%s/%s 가 %s로 등록 되지 않았습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete Success</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Erasing %s/%s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete Failed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Incorrect Erasing %s/%s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제 성공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%s/%s 가 삭제 되었습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제 실패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%s/%s 가 삭제 되지 않았습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Protocol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Allocated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인터페이스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로토콜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할당수치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range Start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range End</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>범위 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>범위 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range Count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>범위 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Utilization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAT Pool Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAT Total Allocated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAT Pool Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAT IPs Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAT Total Allocated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAT 설정 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAT 총 할당 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAT 총 IP 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAT 설정 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAT 총 할당 개수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -711,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1284,6 +1484,356 @@
         <v>80</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:D35">
     <sortCondition ref="A2:A35"/>

</xml_diff>